<commit_message>
Income Page Partially Completed
</commit_message>
<xml_diff>
--- a/Backend/income_details.xlsx
+++ b/Backend/income_details.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Expense" sheetId="1" r:id="rId1"/>
+    <sheet name="Income" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -64,8 +64,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,13 +398,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Source</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Amount</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Date</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>salary</v>
+      </c>
+      <c r="B2">
+        <v>5000</v>
+      </c>
+      <c r="C2" s="1">
+        <v>45879.22928240741</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>salary</v>
+      </c>
+      <c r="B3">
+        <v>50</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45689.22928240741</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>salary</v>
+      </c>
+      <c r="B4">
+        <v>500</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45689.22928240741</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>salary</v>
+      </c>
+      <c r="B5">
+        <v>5000</v>
+      </c>
+      <c r="C5" s="1">
+        <v>45689.22928240741</v>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>